<commit_message>
Handle Don Mua Hang
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/bidv/ĐƠN MUA HÀNG.xlsx
+++ b/adg-api/src/main/resources/bidv/ĐƠN MUA HÀNG.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-api/src/main/resources/bidv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8BDF9D-B3B4-6542-B0C0-710B90499AFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC089321-88EC-4A44-8A99-27CC30E01F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{902AB5DA-4E46-2F4A-81F7-9F513CBA2FD9}"/>
+    <workbookView xWindow="-19200" yWindow="4060" windowWidth="19200" windowHeight="21140" xr2:uid="{902AB5DA-4E46-2F4A-81F7-9F513CBA2FD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Công ty Cổ Phần Á Đông ADG</t>
   </si>
@@ -42,21 +42,12 @@
     <t>ĐƠN MUA HÀNG</t>
   </si>
   <si>
-    <t>CÔNG TY TNHH THƯƠNG MẠI SẢN XUẤT NHỰA NHẬT PHONG</t>
-  </si>
-  <si>
     <t>Địa chỉ</t>
   </si>
   <si>
-    <t>672A29 Phan Văn Trị, Phường 10, Quận Gò Vấp, Thành Phố Hồ Chí Minh, Việt Nam.</t>
-  </si>
-  <si>
     <t>Mã số thuế</t>
   </si>
   <si>
-    <t>0315198603</t>
-  </si>
-  <si>
     <t>Điện thoại</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
     <t>Loại tiền</t>
   </si>
   <si>
-    <t>VND</t>
-  </si>
-  <si>
     <t>Mã hàng</t>
   </si>
   <si>
@@ -87,12 +75,6 @@
     <t>Thành tiền</t>
   </si>
   <si>
-    <t>PP 1100NK</t>
-  </si>
-  <si>
-    <t>Hạt nhựa PP 1100NK</t>
-  </si>
-  <si>
     <t>Thuế suất thuế GTGT</t>
   </si>
   <si>
@@ -105,21 +87,12 @@
     <t>Số tiền viết bằng chữ</t>
   </si>
   <si>
-    <t>Ba tỷ, hai trăm mười bảy triệu, năm trăm nghìn đồng</t>
-  </si>
-  <si>
     <t>Ngày giao hàng</t>
   </si>
   <si>
-    <t>Kể từ ngày 30/04/2022</t>
-  </si>
-  <si>
     <t>Địa điểm giao hàng</t>
   </si>
   <si>
-    <t>Tại kho Công ty Cổ Phần Á Đông ADG</t>
-  </si>
-  <si>
     <t>Điều khoản thanh toán</t>
   </si>
   <si>
@@ -141,19 +114,10 @@
     <t>Tổng tiền</t>
   </si>
   <si>
-    <t>0382582354</t>
-  </si>
-  <si>
     <t>Ngày</t>
   </si>
   <si>
-    <t>30/04/2022</t>
-  </si>
-  <si>
     <t>Số</t>
-  </si>
-  <si>
-    <t>ĐMH220419-04</t>
   </si>
   <si>
     <t>Tên NCC</t>
@@ -395,119 +359,119 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -826,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEEA38B-431B-9045-AD1A-26A80F7A5EAF}">
   <dimension ref="A3:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,125 +806,111 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -968,226 +918,200 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="9" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="21"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="B17" s="25"/>
+      <c r="C17" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E18" s="34"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="E19" s="35"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="35"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B22" s="36"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="10">
-        <v>97500</v>
-      </c>
-      <c r="E15" s="10">
-        <v>30000</v>
-      </c>
-      <c r="F15" s="10">
-        <f>D15*E15</f>
-        <v>2925000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="41"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="40"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="B23" s="36"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37">
-        <f>SUM(F15)</f>
-        <v>2925000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="27" t="s">
+      <c r="B24" s="36"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="26">
-        <f>F17*C17</f>
-        <v>292500000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="25" t="s">
+      <c r="B25" s="36"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26">
-        <f>SUM(F17:F18)</f>
-        <v>3217500000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="B27" s="39"/>
+      <c r="D27" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="25"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="B28" s="38"/>
+      <c r="D28" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="D27" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="D28" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E29" s="24"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:F7"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="A17:B19"/>
     <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:B21"/>
     <mergeCell ref="C20:F21"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>